<commit_message>
delayed CBR start to 5s
</commit_message>
<xml_diff>
--- a/Experiment 3/Trace Files/ThroughputGraph.xlsx
+++ b/Experiment 3/Trace Files/ThroughputGraph.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jae\Documents\CS-5700-Project-3\Experiment 3\Trace Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\akari\OneDrive\Documents\Northeastern\CS 5700\Project 3\Experiment 3\Trace Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="11_BE55D47D0476D648B0AD6F7C5E0360065ECDED8D" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23234" windowHeight="9487"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23235" windowHeight="9488" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -44,7 +45,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -94,7 +95,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -133,7 +134,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -328,6 +328,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-84DF-41B6-9D92-F880266D8C15}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -482,6 +487,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-84DF-41B6-9D92-F880266D8C15}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -533,7 +543,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -654,7 +663,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -729,7 +737,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -797,7 +804,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -836,7 +843,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1031,6 +1037,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-C934-4ECD-8EB9-7519E229A390}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1185,6 +1196,11 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-C934-4ECD-8EB9-7519E229A390}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1236,7 +1252,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1357,7 +1372,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1432,7 +1446,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2628,7 +2641,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -2658,7 +2677,13 @@
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
@@ -2940,16 +2965,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.55" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.45">
       <c r="B1" t="s">
         <v>1</v>
       </c>
@@ -2957,7 +2982,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2974,7 +2999,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A3">
         <v>0.5</v>
       </c>
@@ -2985,7 +3010,7 @@
         <v>410.81165088799997</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2996,7 +3021,7 @@
         <v>413.34302539700002</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A5">
         <v>1.5</v>
       </c>
@@ -3013,7 +3038,7 @@
         <v>737.38067421999995</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A6">
         <v>2</v>
       </c>
@@ -3030,7 +3055,7 @@
         <v>737.49327764700001</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A7">
         <v>2.5</v>
       </c>
@@ -3047,7 +3072,7 @@
         <v>731.11876027300002</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A8">
         <v>3</v>
       </c>
@@ -3064,7 +3089,7 @@
         <v>734.49205967199998</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>3.5</v>
       </c>
@@ -3081,7 +3106,7 @@
         <v>736.08052846800001</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>4</v>
       </c>
@@ -3098,7 +3123,7 @@
         <v>736.00300985299998</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>4.5</v>
       </c>
@@ -3115,7 +3140,7 @@
         <v>736.07853180200004</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>5</v>
       </c>
@@ -3132,7 +3157,7 @@
         <v>736.02571224999997</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>5.5</v>
       </c>
@@ -3149,7 +3174,7 @@
         <v>735.85368461400003</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>6</v>
       </c>
@@ -3166,7 +3191,7 @@
         <v>736.04224051599999</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>6.5</v>
       </c>
@@ -3183,7 +3208,7 @@
         <v>735.93468422399997</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>7</v>
       </c>
@@ -3200,7 +3225,7 @@
         <v>735.94993972899999</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>7.5</v>
       </c>
@@ -3217,7 +3242,7 @@
         <v>735.98097772200003</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>8</v>
       </c>
@@ -3234,7 +3259,7 @@
         <v>735.85766208899997</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>8.5</v>
       </c>
@@ -3251,7 +3276,7 @@
         <v>735.98602490600001</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A20">
         <v>9</v>
       </c>
@@ -3268,7 +3293,7 @@
         <v>735.91665999099996</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>9.5</v>
       </c>

</xml_diff>